<commit_message>
Agrego 2 instrucciones mas para las pruebas, tienen TODOS!
</commit_message>
<xml_diff>
--- a/IDE/docs/traduccion de instrucciones.xlsx
+++ b/IDE/docs/traduccion de instrucciones.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\bluesky-taller-ide\IDE\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="14115" windowHeight="4680"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>1RXY</t>
   </si>
@@ -166,13 +171,40 @@
   </si>
   <si>
     <t>para ejecucion</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>jpc mem</t>
+  </si>
+  <si>
+    <t>If (overflow) goto mem</t>
+  </si>
+  <si>
+    <t>Jump if overflow</t>
+  </si>
+  <si>
+    <t>E0XY</t>
+  </si>
+  <si>
+    <t>DRST</t>
+  </si>
+  <si>
+    <t>reg = reg1 x reg2</t>
+  </si>
+  <si>
+    <t>mulf reg,reg1,reg2</t>
+  </si>
+  <si>
+    <t>Multiplicar fp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +241,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -255,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,9 +327,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,6 +362,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,21 +538,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -544,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -561,7 +603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -575,7 +617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -589,7 +631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -603,7 +645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -617,7 +659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -631,7 +673,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -645,7 +687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -659,7 +701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -673,7 +715,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -685,6 +727,39 @@
       </c>
       <c r="D12" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -693,24 +768,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>